<commit_message>
fix schema and export files
</commit_message>
<xml_diff>
--- a/src/mapex/aws/attack-9.0/aws-09.21.2021/enterprise/aws-09.21.2021_attack-9.0-enterprise.xlsx
+++ b/src/mapex/aws/attack-9.0/aws-09.21.2021/enterprise/aws-09.21.2021_attack-9.0-enterprise.xlsx
@@ -14292,7 +14292,7 @@
       </c>
       <c r="L152" t="inlineStr">
         <is>
-          <t>not_mappable</t>
+          <t>non_mappable</t>
         </is>
       </c>
       <c r="M152" t="inlineStr"/>
@@ -23191,7 +23191,7 @@
       </c>
       <c r="L250" t="inlineStr">
         <is>
-          <t>not_mappable</t>
+          <t>non_mappable</t>
         </is>
       </c>
       <c r="M250" t="inlineStr"/>
@@ -23252,7 +23252,7 @@
       </c>
       <c r="L251" t="inlineStr">
         <is>
-          <t>not_mappable</t>
+          <t>non_mappable</t>
         </is>
       </c>
       <c r="M251" t="inlineStr"/>
@@ -23313,7 +23313,7 @@
       </c>
       <c r="L252" t="inlineStr">
         <is>
-          <t>not_mappable</t>
+          <t>non_mappable</t>
         </is>
       </c>
       <c r="M252" t="inlineStr"/>
@@ -30322,7 +30322,7 @@
       </c>
       <c r="L329" t="inlineStr">
         <is>
-          <t>not_mappable</t>
+          <t>non_mappable</t>
         </is>
       </c>
       <c r="M329" t="inlineStr"/>
@@ -34678,7 +34678,7 @@
       </c>
       <c r="L376" t="inlineStr">
         <is>
-          <t>not_mappable</t>
+          <t>non_mappable</t>
         </is>
       </c>
       <c r="M376" t="inlineStr"/>
@@ -35908,7 +35908,7 @@
       </c>
       <c r="L390" t="inlineStr">
         <is>
-          <t>not_mappable</t>
+          <t>non_mappable</t>
         </is>
       </c>
       <c r="M390" t="inlineStr"/>
@@ -41801,7 +41801,7 @@
       </c>
       <c r="L455" t="inlineStr">
         <is>
-          <t>not_mappable</t>
+          <t>non_mappable</t>
         </is>
       </c>
       <c r="M455" t="inlineStr"/>

</xml_diff>

<commit_message>
Mapex 116 schema updates (#41)
* change mapping type ids from uuids and change 'not_mappable' to 'non_mappable'

* fix schema and export files

* remove unused imports

* add min height of 100vh to the body of the app

* schema updates

* add loading bar, fix broken link, fix terminology

* fix build error

* re-add id and event listeners to navigation

* fill the search value into the input on the search page

* schema updates

* revert changes

---------

Co-authored-by: Eva <emeth.ctr@kr.af.mil>
</commit_message>
<xml_diff>
--- a/src/mapex/aws/attack-9.0/aws-09.21.2021/enterprise/aws-09.21.2021_attack-9.0-enterprise.xlsx
+++ b/src/mapex/aws/attack-9.0/aws-09.21.2021/enterprise/aws-09.21.2021_attack-9.0-enterprise.xlsx
@@ -14292,7 +14292,7 @@
       </c>
       <c r="L152" t="inlineStr">
         <is>
-          <t>not_mappable</t>
+          <t>non_mappable</t>
         </is>
       </c>
       <c r="M152" t="inlineStr"/>
@@ -23191,7 +23191,7 @@
       </c>
       <c r="L250" t="inlineStr">
         <is>
-          <t>not_mappable</t>
+          <t>non_mappable</t>
         </is>
       </c>
       <c r="M250" t="inlineStr"/>
@@ -23252,7 +23252,7 @@
       </c>
       <c r="L251" t="inlineStr">
         <is>
-          <t>not_mappable</t>
+          <t>non_mappable</t>
         </is>
       </c>
       <c r="M251" t="inlineStr"/>
@@ -23313,7 +23313,7 @@
       </c>
       <c r="L252" t="inlineStr">
         <is>
-          <t>not_mappable</t>
+          <t>non_mappable</t>
         </is>
       </c>
       <c r="M252" t="inlineStr"/>
@@ -30322,7 +30322,7 @@
       </c>
       <c r="L329" t="inlineStr">
         <is>
-          <t>not_mappable</t>
+          <t>non_mappable</t>
         </is>
       </c>
       <c r="M329" t="inlineStr"/>
@@ -34678,7 +34678,7 @@
       </c>
       <c r="L376" t="inlineStr">
         <is>
-          <t>not_mappable</t>
+          <t>non_mappable</t>
         </is>
       </c>
       <c r="M376" t="inlineStr"/>
@@ -35908,7 +35908,7 @@
       </c>
       <c r="L390" t="inlineStr">
         <is>
-          <t>not_mappable</t>
+          <t>non_mappable</t>
         </is>
       </c>
       <c r="M390" t="inlineStr"/>
@@ -41801,7 +41801,7 @@
       </c>
       <c r="L455" t="inlineStr">
         <is>
-          <t>not_mappable</t>
+          <t>non_mappable</t>
         </is>
       </c>
       <c r="M455" t="inlineStr"/>

</xml_diff>